<commit_message>
Modified student class import
</commit_message>
<xml_diff>
--- a/import_template/student_class_import_template.xlsx
+++ b/import_template/student_class_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Downloads/excel_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Downloads/voc_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578DE50A-F4AD-B444-8AE0-5CCC281D38F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7054A25-B34A-F24B-A9CF-F23A7673B60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="3840" windowWidth="28660" windowHeight="13700" xr2:uid="{AADB0DC0-6B19-2347-81DE-4E0B5248B355}"/>
+    <workbookView xWindow="540" yWindow="6340" windowWidth="34720" windowHeight="13700" xr2:uid="{AADB0DC0-6B19-2347-81DE-4E0B5248B355}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,28 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
-  <si>
-    <t>class_name</t>
-  </si>
-  <si>
-    <t>instructor_name</t>
-  </si>
-  <si>
-    <t>student_name</t>
-  </si>
-  <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>first_language</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>education</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>French</t>
   </si>
@@ -71,21 +50,9 @@
     <t>Level 1 - Class 5 - Winter</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
     <t>hanqingzhou</t>
   </si>
   <si>
-    <t>CU</t>
-  </si>
-  <si>
-    <t>UO</t>
-  </si>
-  <si>
     <t>Level 1 - Class 6 - Winter</t>
   </si>
   <si>
@@ -102,6 +69,66 @@
   </si>
   <si>
     <t>Buhatel</t>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>Instructor Name</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>123 main st</t>
+  </si>
+  <si>
+    <t>456 main st</t>
+  </si>
+  <si>
+    <t>Carleton University</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>First Language</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>johnsmith</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>789@mail.com</t>
+  </si>
+  <si>
+    <t>1456 main st</t>
   </si>
 </sst>
 </file>
@@ -472,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCB34A2-56E1-C042-B5B0-49895BE0D1BA}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,164 +511,249 @@
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1">
+        <v>123</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>123456</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>456</v>
+      </c>
+      <c r="G3" s="1">
+        <v>456</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <v>456789</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>123</v>
+      </c>
+      <c r="G4" s="1">
+        <v>123</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>123456</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>456</v>
+      </c>
+      <c r="G5" s="1">
+        <v>456</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>456789</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1">
-        <v>123</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>789</v>
+      </c>
+      <c r="G6" s="1">
+        <v>789</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1">
-        <v>456</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1">
-        <v>123</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1">
-        <v>456</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
+      <c r="K6">
+        <v>1456789</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="mailto:123@mail.com" xr:uid="{E0855657-D64A-794F-B2BD-EB7313D6C65E}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{607B1A35-A95B-A74C-9636-0B8D57C37E3F}"/>
-    <hyperlink ref="H4" r:id="rId3" display="mailto:123@mail.com" xr:uid="{A142062E-874D-B848-AC46-E862A881E39F}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{79B8554D-F8B9-104A-A53E-4E23E24E9BDF}"/>
+    <hyperlink ref="I2" r:id="rId1" display="mailto:123@mail.com" xr:uid="{E0855657-D64A-794F-B2BD-EB7313D6C65E}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{607B1A35-A95B-A74C-9636-0B8D57C37E3F}"/>
+    <hyperlink ref="I4" r:id="rId3" display="mailto:123@mail.com" xr:uid="{A142062E-874D-B848-AC46-E862A881E39F}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{79B8554D-F8B9-104A-A53E-4E23E24E9BDF}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{45887BF0-F96A-6A45-948C-F80A39575FC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>